<commit_message>
Full Script minus Conclusion
</commit_message>
<xml_diff>
--- a/deliverables/FinalProject_Script.xlsx
+++ b/deliverables/FinalProject_Script.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e00cfaf0f80ab21d/Documentos/GitHub/MSAAI531/MSAAI521/deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="8_{0B7E1449-FF0E-4D62-A6C9-02AF432541A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC70C14B-9201-47C9-B364-222BEED0FDC3}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="8_{0B7E1449-FF0E-4D62-A6C9-02AF432541A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{374F66E0-FC56-403F-A553-70D4D5726766}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="29010" windowHeight="31785" xr2:uid="{A340C242-620C-4844-A740-5AAB798F6EF1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A340C242-620C-4844-A740-5AAB798F6EF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
   <si>
     <t>Person</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Target</t>
   </si>
   <si>
-    <t>TITLE CARD: CONCLUSION</t>
-  </si>
-  <si>
     <t>Credits</t>
   </si>
   <si>
@@ -303,10 +300,55 @@
   <si>
     <t>NuScenes provides a small version of the dataset, called "nuScenes-panoptic-mini" that contains only 10 scenes, which we used to setup our algorithms. Later on, we downloaded and used the full set for training and testing our methodology.
 We found that each 20-second scene is composed of 404 samples, each one being a snapshot from all sensors captured at 2 Hz, so 2 snapshots of each of the 6 sensors every second. Later on, the team manually entered annotations for the objects on each scene.
-Annotations contain a 3D bounding box describing the class of each object (pedestrian, cyclist, truck, car...), as well as other physical position features like translation, size, and rotation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TITLE CARD: </t>
+Annotations contain a 3D bounding box describing the class of each object (pedestrian, cyclist, truck, car...), as well as other physical position features like translation, size, and rotation. These annotations will be helpful to confirm if the predictions from the model are correct.</t>
+  </si>
+  <si>
+    <t>TITLE CARD: Data Preprocessing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The vehicle carrying the sensors is called the "ego" vehicle, to distinguish it from all other vehicles on the scene as the "self" vehicle.
+Our goal is to predict the annotated classes and their locations in each frame, which would allow the self-driving ego vehicle to make real-time decisions. For those predictions, we have selected the YOLO model, which stands for "You Only Look Once", and is a proven algorithm that extracts features out of a two-dimensional image in a very short amount of time.
+So, our next step is to convert the LiDAR three-dimensional information into two-dimensional images that the YOLO model can use. This is a critical step before any predictions can be made.
+Lidar range can reach long distances, so we've decided to limit the processing to data within a range of 100 meters around the vehicle (about 328ft). This filtering reduces computational load by 50-70% while retaining all relevant objects for autonomous driving perception. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The core innovation of our approach is converting 3D point clouds into 2D BEV images that encode spatial information in multiple channels. The colors on the images won't technically represent real colors, but rather each RGB channel represents dimensions to be used by the YOLO model: height of the cloud point, intensity, and density.
+For each frame in a scene, we created a standard PNG image of 1000 by 1000 pixels (although later we adjusted the resolution to 1280 by 1280 and had a significantly better performance). </t>
+  </si>
+  <si>
+    <t>TITLE CARD: The Model</t>
+  </si>
+  <si>
+    <t>Additionally, nuScenes has annotations of of 23 categories, that's 23 different types of objects. We decided to simplify it and consolidate only into these 4 classes:
+- Class 0: Cars (standard household cars, taxi cabs, etc)
+- Class 1: Trucks/Buses (large vehicles like fire trucks, buses, construction vehicles)
+- Class 2: Pedestrians (people walking)
+- Class 3: Cyclists (bicycles, motorcycles, and other similar smaller vehicles)
+This reduces class imbalance and focuses on key autonomous driving objects, simplifying the processing for the model.</t>
+  </si>
+  <si>
+    <t>We decided to use YOLO version 12s, a small variants of the current YOLO 12 version, as the base for our prediction. This version has over 9 million parameters, which is trainable on a relatively small computer. 
+We are also using a pre-trained COCO weights, which provide a strong low-level feature extraction (like edges, textures, and shapes). Since the COCO weighs were trained on regular RGB images, we'll have to re-train it and adjust it to our LiDAR-based images with a two-stage training approach.</t>
+  </si>
+  <si>
+    <t>TITLE CARD: The Results</t>
+  </si>
+  <si>
+    <t>Let's define first the metrics we'll use to measure the performance.
+Precision represents how many of the predictions were actually correct; for example, if from the 10 predicted pedestrians, 8 are actually pedestrians, the precision would be 80%.
+Recall measures from the total possible predictions, how many were successfully identified by the model; for instance, if out of the 12 real pedestrians the model identified 8, the recall would be 66%.
+Next, comes the Mean Average Precision (mAP) is very specific for box predictions. We want to measure how much our predicted box with the location and measurement of the object aligns with the annotated box. We have the mAP in 2 versions: mAP50, which measures how many of the boxes overlap with their annotations by at least 50%, while mAP50-95 measures how many boxes almost perfectly match the annotations (up to 95% overlap).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+On the first stage, which we called "The Warmup", the model trained for 50 epochs, and prepared the initial COCO weights for the long second phase: "The Fine Tunning", in which the weights get readjusted for 150 epochs.
+We experimented several times on different computer environments with GPUs. One of our biggest challenges was running time -  even if we were using GPUs, the full training took over one hour, and for our last run in which we increased the resolution of the images from the initial 1000 by 1000 up to 1280 by 1280. The final results were astounding.</t>
+  </si>
+  <si>
+    <t>Overall, the precision of the training set was 66%, with a recall of only 41%. Then we tested the model with previously unseen data, and got it to perform at 81% precision and 39% recall.
+When it comes to mAP50, the testing set got to 45% while the much stricter mAP50-95 got to 26%, while the validation set achieved 62% and 38%, respectively. 
+It's very important to measure the performance from the perspective of each of the 4 classes to identify if there are any objects harder to detect by the model.
+We found that Cars and Trucks have the best performance with a precision of 86% and 77%, respectively, while smaller objects like Pedestrians and Cyclists got a precision of 71% and 88%. However, Cyclists are showing the lowest recall of only 10%, meaning that 90% of the cyclists were not predicted by the model. This is still an area of opportunity of our project.</t>
   </si>
 </sst>
 </file>
@@ -677,7 +719,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -775,9 +817,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -813,15 +852,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -839,6 +869,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -864,6 +895,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -871,6 +903,15 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -933,22 +974,22 @@
     <tableColumn id="1" xr3:uid="{4BE4823E-1F82-4833-AF2F-131DD010580C}" name="Person"/>
     <tableColumn id="2" xr3:uid="{DB562737-07D7-4E32-87BE-737A9E467551}" name="Script"/>
     <tableColumn id="3" xr3:uid="{82DA99BE-8FA5-418D-8B10-AB213BBA6A87}" name="Manual Duration" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{8B62B8E7-2869-4C2D-B8C8-CC3A3287E19F}" name="Word Count" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{8B62B8E7-2869-4C2D-B8C8-CC3A3287E19F}" name="Word Count" dataDxfId="0">
       <calculatedColumnFormula>IF(LEN(TRIM(C3))=0,0,LEN(TRIM(C3))-LEN(SUBSTITUTE(C3," ",""))+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E3108AD1-6EE7-4AC3-8709-A0CD4E39F2D5}" name="Calc Duration" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{E3108AD1-6EE7-4AC3-8709-A0CD4E39F2D5}" name="Calc Duration" dataDxfId="5">
       <calculatedColumnFormula>IF(B3="",5,ROUND(E3/$C$1,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{323E07CE-ED8A-4368-BB59-A5DB12DB9DCF}" name="Considered Duration" dataDxfId="3">
-      <calculatedColumnFormula>IF(C3="",0, IF(D3="",F3,D3))</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{323E07CE-ED8A-4368-BB59-A5DB12DB9DCF}" name="Considered Duration" dataDxfId="1">
+      <calculatedColumnFormula>IF(C4="",0, IF(D3="",F3,D3))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{56248789-C177-4452-98BA-F0B1F351C871}" name="Cumul." dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{56248789-C177-4452-98BA-F0B1F351C871}" name="Cumul." dataDxfId="4">
       <calculatedColumnFormula>IF(D3="",F3,D3)+H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{17F3D273-F25E-4785-8267-E7D2BFF55085}" name="Min" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{17F3D273-F25E-4785-8267-E7D2BFF55085}" name="Min" dataDxfId="3">
       <calculatedColumnFormula>FLOOR(H3/60,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4B0D3E92-9097-41DC-A6A4-18D516858FE4}" name="Sec" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{4B0D3E92-9097-41DC-A6A4-18D516858FE4}" name="Sec" dataDxfId="2">
       <calculatedColumnFormula>H3-I3*60</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1276,10 +1317,10 @@
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,28 +1347,28 @@
       </c>
       <c r="E1" s="27">
         <f>SUMIFS(Table1[[#All],[Considered Duration]],Table1[[#All],[Person]],D1)/$M$1</f>
-        <v>0.36499999999999999</v>
+        <v>0.35672514619883039</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G1" s="27">
         <f>SUMIFS(Table1[[#All],[Considered Duration]],Table1[[#All],[Person]],F1)/$M$1</f>
-        <v>0.32</v>
+        <v>0.30701754385964913</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I1" s="27">
         <f>SUMIFS(Table1[[#All],[Considered Duration]],Table1[[#All],[Person]],H1)/$M$1</f>
-        <v>0.19</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="L1" s="28" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="29">
         <f>SUM(Table1[[#All],[Considered Duration]])</f>
-        <v>400</v>
+        <v>684</v>
       </c>
       <c r="N1" s="30"/>
       <c r="O1" s="28" t="s">
@@ -1335,20 +1376,20 @@
       </c>
       <c r="P1" s="29">
         <f>FLOOR(M1/60,1)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="Q1" s="28" t="s">
         <v>6</v>
       </c>
       <c r="R1" s="29">
         <f>$M$1-P1*60</f>
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="S1" s="30"/>
     </row>
     <row r="2" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>0</v>
@@ -1410,15 +1451,15 @@
         <v>5</v>
       </c>
       <c r="E3" s="31">
-        <f>IF(LEN(TRIM(C3))=0,0,LEN(TRIM(C3))-LEN(SUBSTITUTE(C3," ",""))+1)</f>
+        <f t="shared" ref="E3:E35" si="0">IF(LEN(TRIM(C3))=0,0,LEN(TRIM(C3))-LEN(SUBSTITUTE(C3," ",""))+1)</f>
         <v>6</v>
       </c>
       <c r="F3" s="31">
-        <f t="shared" ref="F3:F35" si="0">IF(B3="",5,ROUND(E3/$C$1,0))</f>
+        <f t="shared" ref="F3:F35" si="1">IF(B3="",5,ROUND(E3/$C$1,0))</f>
         <v>5</v>
       </c>
       <c r="G3" s="31">
-        <f>IF(C3="",0, IF(D3="",F3,D3))</f>
+        <f t="shared" ref="G3:G35" si="2">IF(C4="",0, IF(D3="",F3,D3))</f>
         <v>5</v>
       </c>
       <c r="H3" s="32">
@@ -1443,19 +1484,19 @@
         <v>3</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="31">
-        <f t="shared" ref="E4:E34" si="1">IF(LEN(TRIM(C4))=0,0,LEN(TRIM(C4))-LEN(SUBSTITUTE(C4," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
       <c r="F4" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="G4" s="31">
-        <f t="shared" ref="G4:G35" si="2">IF(C4="",0, IF(D4="",F4,D4))</f>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="H4" s="32">
@@ -1478,17 +1519,17 @@
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" s="31">
         <v>5</v>
       </c>
       <c r="E5" s="31">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F5" s="31">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="F5" s="31">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G5" s="31">
@@ -1514,18 +1555,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="31">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F6" s="31">
         <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="F6" s="31">
-        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="G6" s="31">
@@ -1552,17 +1593,17 @@
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="31">
         <v>5</v>
       </c>
       <c r="E7" s="31">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F7" s="31">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F7" s="31">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G7" s="31">
@@ -1595,18 +1636,18 @@
         <v>6</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="31">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="F8" s="31">
         <f t="shared" si="1"/>
-        <v>54</v>
-      </c>
-      <c r="F8" s="31">
-        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="G8" s="31">
@@ -1642,15 +1683,15 @@
         <v>3</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="31">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="F9" s="31">
         <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="F9" s="31">
-        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="G9" s="31">
@@ -1680,18 +1721,18 @@
         <v>8</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="31">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F10" s="31">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="F10" s="31">
-        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="G10" s="31">
@@ -1718,17 +1759,17 @@
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" s="16">
         <v>5</v>
       </c>
       <c r="E11" s="31">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F11" s="31">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="F11" s="31">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G11" s="31">
@@ -1760,15 +1801,15 @@
         <v>3</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="F12" s="31">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="F12" s="31">
-        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="G12" s="31">
@@ -1798,18 +1839,18 @@
         <v>11</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="31">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F13" s="31">
         <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="F13" s="31">
-        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="G13" s="31">
@@ -1839,18 +1880,18 @@
         <v>12</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="31">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="F14" s="31">
         <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="F14" s="31">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="G14" s="31">
@@ -1881,17 +1922,17 @@
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="16">
         <v>5</v>
       </c>
       <c r="E15" s="31">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F15" s="31">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="F15" s="31">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G15" s="31">
@@ -1917,18 +1958,18 @@
         <v>14</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="31">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="F16" s="31">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="F16" s="31">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="G16" s="31">
@@ -1948,24 +1989,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="31">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="F17" s="31">
         <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="F17" s="31">
-        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="G17" s="31">
@@ -1985,23 +2026,23 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="31">
         <v>5</v>
       </c>
       <c r="E18" s="31">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F18" s="31">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F18" s="31">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G18" s="31">
@@ -2021,7 +2062,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="189" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="189" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="5"/>
         <v>17</v>
@@ -2030,15 +2071,15 @@
         <v>3</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="31">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+      <c r="F19" s="31">
         <f t="shared" si="1"/>
-        <v>116</v>
-      </c>
-      <c r="F19" s="31">
-        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="G19" s="31">
@@ -2058,33 +2099,33 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="189" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" s="31"/>
       <c r="E20" s="31">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="F20" s="31">
         <f t="shared" si="1"/>
-        <v>110</v>
-      </c>
-      <c r="F20" s="31">
-        <f t="shared" si="0"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G20" s="31">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H20" s="32">
         <f t="shared" si="6"/>
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="I20" s="32">
         <f t="shared" si="9"/>
@@ -2092,34 +2133,35 @@
       </c>
       <c r="J20" s="32">
         <f t="shared" si="10"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="B21" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="31"/>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="31">
+        <v>5</v>
+      </c>
       <c r="E21" s="31">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F21" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G21" s="31">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H21" s="32">
         <f t="shared" si="6"/>
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="I21" s="32">
         <f t="shared" si="9"/>
@@ -2127,198 +2169,214 @@
       </c>
       <c r="J21" s="32">
         <f t="shared" si="10"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="B22" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>82</v>
+      </c>
       <c r="D22" s="31"/>
       <c r="E22" s="31">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="F22" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="31">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="G22" s="31">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="H22" s="32">
         <f t="shared" si="6"/>
-        <v>380</v>
+        <v>458</v>
       </c>
       <c r="I22" s="32">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J22" s="32">
         <f t="shared" si="10"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="M22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="126" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
-      <c r="C23" t="s">
-        <v>82</v>
+      <c r="B23" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="31">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="F23" s="31">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F23" s="31">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="G23" s="31">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="H23" s="32">
         <f t="shared" si="6"/>
-        <v>385</v>
+        <v>495</v>
       </c>
       <c r="I23" s="32">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J23" s="32">
         <f t="shared" si="10"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="5"/>
         <v>22</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="25"/>
+      <c r="B24" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>85</v>
+      </c>
       <c r="D24" s="32"/>
       <c r="E24" s="31">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="F24" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="G24" s="31">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="H24" s="32">
         <f t="shared" si="6"/>
-        <v>385</v>
+        <v>528</v>
       </c>
       <c r="I24" s="32">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J24" s="32">
         <f t="shared" si="10"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="5"/>
         <v>23</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="32"/>
+      <c r="C25" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="32">
+        <v>5</v>
+      </c>
       <c r="E25" s="31">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F25" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G25" s="31">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H25" s="32">
         <f t="shared" si="6"/>
-        <v>385</v>
+        <v>533</v>
       </c>
       <c r="I25" s="32">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J25" s="32">
         <f t="shared" si="10"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="126" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="34"/>
+        <v>63</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>86</v>
+      </c>
       <c r="D26" s="33"/>
       <c r="E26" s="31">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="F26" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="G26" s="31">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H26" s="32">
         <f t="shared" si="6"/>
-        <v>385</v>
+        <v>570</v>
       </c>
       <c r="I26" s="32">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J26" s="32">
         <f t="shared" si="10"/>
-        <v>25</v>
-      </c>
-      <c r="K26" s="21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="K26" s="21"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="5"/>
         <v>25</v>
       </c>
-      <c r="C27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="33"/>
+      <c r="C27" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="32">
+        <v>5</v>
+      </c>
       <c r="E27" s="31">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F27" s="31">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F27" s="31">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G27" s="31">
@@ -2327,21 +2385,19 @@
       </c>
       <c r="H27" s="32">
         <f t="shared" si="6"/>
-        <v>390</v>
+        <v>575</v>
       </c>
       <c r="I27" s="32">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J27" s="32">
         <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-      <c r="K27" s="21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="K27" s="21"/>
+    </row>
+    <row r="28" spans="1:13" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="5"/>
         <v>26</v>
@@ -2349,107 +2405,111 @@
       <c r="B28" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="34"/>
+      <c r="C28" s="17" t="s">
+        <v>88</v>
+      </c>
       <c r="D28" s="33"/>
       <c r="E28" s="31">
+        <f t="shared" si="0"/>
+        <v>141</v>
+      </c>
+      <c r="F28" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="G28" s="31">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="H28" s="32">
         <f t="shared" si="6"/>
-        <v>390</v>
+        <v>636</v>
       </c>
       <c r="I28" s="32">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J28" s="32">
         <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-      <c r="K28" s="21">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="K28" s="21"/>
+    </row>
+    <row r="29" spans="1:13" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="25"/>
+        <v>62</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>89</v>
+      </c>
       <c r="D29" s="32"/>
       <c r="E29" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>99</v>
       </c>
       <c r="F29" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="F29:F35" si="11">IF(B29="",5,ROUND(E29/$C$1,0))</f>
+        <v>43</v>
       </c>
       <c r="G29" s="31">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="H29" s="32">
-        <f t="shared" si="6"/>
-        <v>390</v>
+        <f t="shared" ref="H29:H35" si="12">G29+H28</f>
+        <v>679</v>
       </c>
       <c r="I29" s="32">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" ref="I29:I35" si="13">FLOOR(H29/60,1)</f>
+        <v>11</v>
       </c>
       <c r="J29" s="32">
-        <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J29:J35" si="14">H29-I29*60</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="25"/>
+        <v>63</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>90</v>
+      </c>
       <c r="D30" s="32"/>
       <c r="E30" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>154</v>
       </c>
       <c r="F30" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>67</v>
       </c>
       <c r="G30" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H30" s="32">
-        <f t="shared" si="6"/>
-        <v>390</v>
+        <f t="shared" si="12"/>
+        <v>679</v>
       </c>
       <c r="I30" s="32">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" si="13"/>
+        <v>11</v>
       </c>
       <c r="J30" s="32">
-        <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="5"/>
         <v>29</v>
@@ -2457,14 +2517,14 @@
       <c r="B31" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="25"/>
+      <c r="C31" s="17"/>
       <c r="D31" s="32"/>
       <c r="E31" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F31" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G31" s="31">
@@ -2472,33 +2532,33 @@
         <v>0</v>
       </c>
       <c r="H31" s="32">
-        <f t="shared" si="6"/>
-        <v>390</v>
+        <f t="shared" si="12"/>
+        <v>679</v>
       </c>
       <c r="I31" s="32">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" si="13"/>
+        <v>11</v>
       </c>
       <c r="J31" s="32">
-        <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="14"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="C32" s="25" t="s">
-        <v>67</v>
+      <c r="C32" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="D32" s="32"/>
       <c r="E32" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F32" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="G32" s="31">
@@ -2506,16 +2566,16 @@
         <v>5</v>
       </c>
       <c r="H32" s="32">
-        <f t="shared" si="6"/>
-        <v>395</v>
+        <f t="shared" si="12"/>
+        <v>684</v>
       </c>
       <c r="I32" s="32">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" si="13"/>
+        <v>11</v>
       </c>
       <c r="J32" s="32">
-        <f t="shared" si="10"/>
-        <v>35</v>
+        <f t="shared" si="14"/>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2523,44 +2583,44 @@
         <f t="shared" si="5"/>
         <v>31</v>
       </c>
-      <c r="C33" s="25" t="s">
-        <v>38</v>
+      <c r="C33" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="D33" s="32"/>
       <c r="E33" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F33" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="G33" s="31">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H33" s="32">
-        <f t="shared" si="6"/>
-        <v>400</v>
+        <f t="shared" si="12"/>
+        <v>684</v>
       </c>
       <c r="I33" s="32">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" si="13"/>
+        <v>11</v>
       </c>
       <c r="J33" s="32">
-        <f t="shared" si="10"/>
-        <v>40</v>
+        <f t="shared" si="14"/>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C34" s="17"/>
       <c r="D34" s="31"/>
       <c r="E34" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F34" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="G34" s="31">
@@ -2568,27 +2628,27 @@
         <v>0</v>
       </c>
       <c r="H34" s="32">
-        <f t="shared" si="6"/>
-        <v>400</v>
+        <f t="shared" si="12"/>
+        <v>684</v>
       </c>
       <c r="I34" s="32">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" si="13"/>
+        <v>11</v>
       </c>
       <c r="J34" s="32">
-        <f t="shared" si="10"/>
-        <v>40</v>
+        <f t="shared" si="14"/>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C35" s="25"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="32"/>
       <c r="E35" s="31">
-        <f t="shared" ref="E35" si="11">IF(LEN(TRIM(C35))=0,0,LEN(TRIM(C35))-LEN(SUBSTITUTE(C35," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F35" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="G35" s="31">
@@ -2596,16 +2656,16 @@
         <v>0</v>
       </c>
       <c r="H35" s="32">
-        <f t="shared" si="6"/>
-        <v>400</v>
+        <f t="shared" si="12"/>
+        <v>684</v>
       </c>
       <c r="I35" s="32">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" si="13"/>
+        <v>11</v>
       </c>
       <c r="J35" s="32">
-        <f t="shared" si="10"/>
-        <v>40</v>
+        <f t="shared" si="14"/>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2716,27 +2776,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="40" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="40" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="41"/>
-      <c r="J1" s="43"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
+      <c r="A2" s="38"/>
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
@@ -3082,21 +3142,21 @@
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44" t="s">
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
     </row>
     <row r="2" spans="1:15" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -3128,7 +3188,7 @@
         <v>14</v>
       </c>
       <c r="O2" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
@@ -3448,147 +3508,147 @@
   <sheetData>
     <row r="1" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="F1" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="35" t="s">
+      <c r="B2" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="35" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="34">
+        <v>0</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="35">
+        <v>0.85071099999999999</v>
+      </c>
+      <c r="D3" s="35">
+        <v>0.84849200000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="34">
+        <v>1</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="35">
+        <v>0.92417099999999996</v>
+      </c>
+      <c r="D4" s="35">
+        <v>0.92442299999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="34">
+        <v>2</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="35">
+        <v>0.90995300000000001</v>
+      </c>
+      <c r="D5" s="35">
+        <v>0.909223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="34">
+        <v>3</v>
+      </c>
+      <c r="B6" s="35" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="35">
-        <v>0</v>
-      </c>
-      <c r="B3" s="36" t="s">
+      <c r="C6" s="35">
+        <v>0.92891000000000001</v>
+      </c>
+      <c r="D6" s="35">
+        <v>0.92820199999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="34">
+        <v>4</v>
+      </c>
+      <c r="B7" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="36">
-        <v>0.85071099999999999</v>
-      </c>
-      <c r="D3" s="36">
-        <v>0.84849200000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="35">
-        <v>1</v>
-      </c>
-      <c r="B4" s="36" t="s">
+      <c r="C7" s="35">
+        <v>0.32227499999999998</v>
+      </c>
+      <c r="D7" s="35">
+        <v>0.19963400000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="34">
+        <v>5</v>
+      </c>
+      <c r="B8" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="36">
-        <v>0.92417099999999996</v>
-      </c>
-      <c r="D4" s="36">
-        <v>0.92442299999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="35">
-        <v>2</v>
-      </c>
-      <c r="B5" s="36" t="s">
+      <c r="C8" s="35">
+        <v>0.919431</v>
+      </c>
+      <c r="D8" s="35">
+        <v>0.91874400000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="34">
+        <v>6</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="35">
+        <v>0.85545000000000004</v>
+      </c>
+      <c r="D9" s="35">
+        <v>0.855518</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="34">
+        <v>7</v>
+      </c>
+      <c r="B10" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C10" s="35">
         <v>0.90995300000000001</v>
       </c>
-      <c r="D5" s="36">
-        <v>0.909223</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="35">
-        <v>3</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="36">
-        <v>0.92891000000000001</v>
-      </c>
-      <c r="D6" s="36">
-        <v>0.92820199999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="35">
-        <v>4</v>
-      </c>
-      <c r="B7" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="36">
-        <v>0.32227499999999998</v>
-      </c>
-      <c r="D7" s="36">
-        <v>0.19963400000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="35">
-        <v>5</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="36">
-        <v>0.919431</v>
-      </c>
-      <c r="D8" s="36">
-        <v>0.91874400000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="35">
-        <v>6</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="36">
-        <v>0.85545000000000004</v>
-      </c>
-      <c r="D9" s="36">
-        <v>0.855518</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="35">
-        <v>7</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="36">
-        <v>0.90995300000000001</v>
-      </c>
-      <c r="D10" s="36">
+      <c r="D10" s="35">
         <v>0.91030500000000003</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
         <v>52</v>
       </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -3599,12 +3659,12 @@
         <v>0.96</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="37">
+        <v>53</v>
+      </c>
+      <c r="G17" s="36">
         <v>0.97</v>
       </c>
     </row>
@@ -3616,12 +3676,12 @@
         <v>0.96</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="37">
+        <v>54</v>
+      </c>
+      <c r="G18" s="36">
         <v>0.96</v>
       </c>
     </row>
@@ -3633,12 +3693,12 @@
         <v>0.96</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="37">
+        <v>55</v>
+      </c>
+      <c r="G19" s="36">
         <v>0.95</v>
       </c>
     </row>

</xml_diff>